<commit_message>
fixed problem of foreign keys
</commit_message>
<xml_diff>
--- a/database/thesis-internal-co-supervisors.xlsx
+++ b/database/thesis-internal-co-supervisors.xlsx
@@ -40,7 +40,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -398,7 +398,7 @@
     <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -406,7 +406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -414,7 +414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
         <v>1</v>
       </c>

</xml_diff>